<commit_message>
Added some random interests to correct profile for Sarah Wald
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Sarah_Wald/Author_form.xlsx
+++ b/website_content_creation/authors/Sarah_Wald/Author_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Sarah_Wald/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60C16FDF-28EC-4FA8-A966-3019321F7D11}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7374881A-F3BB-45F0-9769-9109921EEA82}"/>
   <bookViews>
-    <workbookView xWindow="-14235" yWindow="-16395" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Ecosystem change group</t>
+  </si>
+  <si>
+    <t>Hiking</t>
+  </si>
+  <si>
+    <t>Outdoors</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -567,15 +573,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -586,7 +583,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -806,7 +811,7 @@
   <dimension ref="A1:C1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -850,7 +855,7 @@
       <c r="A5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="29" t="s">
         <v>32</v>
       </c>
     </row>
@@ -858,7 +863,7 @@
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="30" t="s">
         <v>33</v>
       </c>
     </row>
@@ -872,7 +877,7 @@
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="31" t="s">
         <v>34</v>
       </c>
     </row>
@@ -925,7 +930,7 @@
       <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C15" t="s">
@@ -938,11 +943,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
@@ -956,13 +961,13 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="33" t="s">
         <v>37</v>
       </c>
     </row>
@@ -988,10 +993,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="32"/>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
@@ -1002,10 +1007,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="31" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1040,10 +1045,14 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="25" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="26"/>

</xml_diff>

<commit_message>
Corrected Sarah Wald profile
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Sarah_Wald/Author_form.xlsx
+++ b/website_content_creation/authors/Sarah_Wald/Author_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Sarah_Wald/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7374881A-F3BB-45F0-9769-9109921EEA82}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EB1689D-D43F-4A40-8BAF-14011FB2BBD8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -117,15 +117,6 @@
     <t>Sarah Wald</t>
   </si>
   <si>
-    <t>Summer intern</t>
-  </si>
-  <si>
-    <t>Watershed Ecology Team</t>
-  </si>
-  <si>
-    <t>instagram.com/sarahwald_</t>
-  </si>
-  <si>
     <t>sw2108@cam.ac.uk</t>
   </si>
   <si>
@@ -141,16 +132,22 @@
     <t>2023-2026</t>
   </si>
   <si>
-    <t>ecosystemchange.com</t>
-  </si>
-  <si>
-    <t>Ecosystem change group</t>
-  </si>
-  <si>
     <t>Hiking</t>
   </si>
   <si>
     <t>Outdoors</t>
+  </si>
+  <si>
+    <t>www.cam.ac.uk</t>
+  </si>
+  <si>
+    <t>www.instagram.com/sarahwald_/</t>
+  </si>
+  <si>
+    <t>Summer intern, University of Cambridge</t>
+  </si>
+  <si>
+    <t>Visiting and Co-supervised Students</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -576,7 +573,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -810,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -845,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -856,15 +852,15 @@
         <v>28</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>33</v>
+      <c r="B6" s="29" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -877,8 +873,8 @@
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>34</v>
+      <c r="B8" s="30" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,7 +927,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -943,11 +939,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
@@ -961,14 +957,14 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>37</v>
+      <c r="A19" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -993,10 +989,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="38"/>
+      <c r="B25" s="37"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
@@ -1008,10 +1004,10 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1046,12 +1042,12 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2035,9 +2031,11 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{24DD6C1B-E536-4334-808A-E7EADF817A76}"/>
     <hyperlink ref="B8" r:id="rId2" xr:uid="{3D731F34-0BCD-40A7-BCD2-8E0A41DD138F}"/>
+    <hyperlink ref="B27" r:id="rId3" xr:uid="{20A7EFB0-F2FE-4562-B9B4-17C42F87F641}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{DA79B313-5540-42C7-BAE8-00A2B1828915}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 UNCLASSIFIED - NON CLASSIFIÉ&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Cambridge University wording consistency
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Sarah_Wald/Author_form.xlsx
+++ b/website_content_creation/authors/Sarah_Wald/Author_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Sarah_Wald/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\OneDrive - NRCan RNCan\Documents\WET lab\GLFC-WET.github.io\website_content_creation\authors\Sarah_Wald\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EB1689D-D43F-4A40-8BAF-14011FB2BBD8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DB1795-5C45-45A3-A57C-B350D55E3C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>Undergraduate</t>
   </si>
   <si>
-    <t>Cambridge University</t>
-  </si>
-  <si>
     <t>2023-2026</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Visiting and Co-supervised Students</t>
+  </si>
+  <si>
+    <t>University of Cambridge</t>
   </si>
 </sst>
 </file>
@@ -807,7 +807,7 @@
   <dimension ref="A1:C1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -852,7 +852,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -927,7 +927,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -961,10 +961,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="32" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1004,10 +1004,10 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1042,12 +1042,12 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>